<commit_message>
correcoes ac04 christiane - atender cliente
</commit_message>
<xml_diff>
--- a/docs/ARTEFATOS(15-23)/ATENDER_CLIENTE/Analise_de_Eventos_ATENDER_CLIENTE.xlsx
+++ b/docs/ARTEFATOS(15-23)/ATENDER_CLIENTE/Analise_de_Eventos_ATENDER_CLIENTE.xlsx
@@ -84,7 +84,7 @@
     <t xml:space="preserve">A cozinha informa que o pedido está pronto</t>
   </si>
   <si>
-    <t xml:space="preserve">O cliente solicita o fechamento do pedido</t>
+    <t xml:space="preserve">O copeiro entrega a bebida solicitada</t>
   </si>
 </sst>
 </file>
@@ -351,7 +351,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>